<commit_message>
update MS Access and PowerBI file for Chi Nhanh and Khu Vuc
</commit_message>
<xml_diff>
--- a/2023-NHA-TRANG-Data-Analytics-for-Managers/Bao-Hiem/raw/1-RM-Ha.xlsx
+++ b/2023-NHA-TRANG-Data-Analytics-for-Managers/Bao-Hiem/raw/1-RM-Ha.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\Lectures\2023-NHA-TRANG-Data-Analytics-for-Managers\Bao-Hiem\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD2A70C-A681-4791-83D6-4D995F740763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{679FD83E-3485-4AF6-8E51-D15D0C1D34D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-8550" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{10B5EDF1-7213-4714-A16C-DAF877EE2D0B}"/>
+    <workbookView xWindow="28680" yWindow="-8550" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{10B5EDF1-7213-4714-A16C-DAF877EE2D0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sale" sheetId="3" r:id="rId1"/>
@@ -34,6 +34,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">DAO!$A$1:$C$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'RM HÀ'!$A$4:$AB$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sale!$A$3:$X$3</definedName>
     <definedName name="asd" localSheetId="7">OFFSET(#REF!,0,0,COUNTA(#REF! )-COUNTIF(#REF!,""),1)</definedName>
     <definedName name="asd">OFFSET(#REF!,0,0,COUNTA(#REF! )-COUNTIF(#REF!,""),1)</definedName>
     <definedName name="BPHI_DT">"BPHI_DT"</definedName>
@@ -7153,7 +7154,7 @@
   <dimension ref="A1:X95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14130,6 +14131,7 @@
       <c r="V95" s="128"/>
     </row>
   </sheetData>
+  <autoFilter ref="A3:X3" xr:uid="{A7F5BDE1-79EF-4352-BFE4-88CF34869C41}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -15304,7 +15306,7 @@
   <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="N2" sqref="N2:N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15313,6 +15315,7 @@
     <col min="5" max="5" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -15462,6 +15465,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -15535,7 +15539,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63DE2D23-AA3D-423C-89A2-5CCFA1B7414D}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -35744,7 +35750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19CAA592-D3A8-4BAE-B7C1-71D59CB3BDDE}">
   <dimension ref="A1:D126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>

</xml_diff>